<commit_message>
gave meaningful column names and table names.
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533711\Desktop\Semester 2\C# .NET\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533490\Documents\44663\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -59,12 +59,6 @@
     <t>MS ACS + DB</t>
   </si>
   <si>
-    <t>DegreeAbbrev (U, B)</t>
-  </si>
-  <si>
-    <t>DegreeName (U, 20)</t>
-  </si>
-  <si>
     <t>NumberOfTerms</t>
   </si>
   <si>
@@ -313,6 +307,12 @@
   </si>
   <si>
     <t>Fall 2018 fast track</t>
+  </si>
+  <si>
+    <t>DegreeAbbrev</t>
+  </si>
+  <si>
+    <t>DegreeName</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,16 +744,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="E1" s="14">
         <v>919</v>
@@ -761,16 +761,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="7">
         <v>919571565</v>
@@ -778,16 +778,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="7">
         <v>919568899</v>
@@ -795,16 +795,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="7">
         <v>919570594</v>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -944,22 +944,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,10 +967,10 @@
         <v>460</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -987,10 +987,10 @@
         <v>356</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -1010,7 +1010,7 @@
         <v>542</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -1030,7 +1030,7 @@
         <v>563</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -1050,7 +1050,7 @@
         <v>560</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -1067,10 +1067,10 @@
         <v>664</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -1087,10 +1087,10 @@
         <v>618</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -1107,10 +1107,10 @@
         <v>555</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -1127,10 +1127,10 @@
         <v>691</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1147,10 +1147,10 @@
         <v>692</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1167,10 +1167,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -1187,10 +1187,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -1207,10 +1207,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1247,13 +1247,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,16 +1807,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1824,13 +1824,13 @@
         <v>7250</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1838,13 +1838,13 @@
         <v>7251</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1852,13 +1852,13 @@
         <v>7252</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,13 +1866,13 @@
         <v>7253</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,13 +1880,13 @@
         <v>7254</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1894,13 +1894,13 @@
         <v>7255</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1927,19 +1927,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1947,16 +1947,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1964,16 +1964,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="8">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1981,16 +1981,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,16 +1998,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="8">
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2015,16 +2015,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="8">
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,16 +2032,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2049,16 +2049,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="10">
         <v>2</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2066,16 +2066,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2083,16 +2083,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="10">
         <v>4</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2100,16 +2100,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="10">
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2117,16 +2117,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="10">
         <v>6</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2134,16 +2134,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" s="12">
         <v>1</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2151,16 +2151,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="12">
         <v>2</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2168,16 +2168,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" s="12">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2185,16 +2185,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="12">
         <v>4</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2202,16 +2202,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="12">
         <v>5</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2219,16 +2219,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="12">
         <v>6</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2256,19 +2256,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2286,7 +2286,7 @@
         <v>460</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -2304,7 +2304,7 @@
         <v>542</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2322,7 +2322,7 @@
         <v>563</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2340,7 +2340,7 @@
         <v>560</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2358,7 +2358,7 @@
         <v>664</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2376,7 +2376,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2394,7 +2394,7 @@
         <v>618</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2412,7 +2412,7 @@
         <v>691</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2430,7 +2430,7 @@
         <v>692</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2448,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -2466,7 +2466,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2484,7 +2484,7 @@
         <v>555</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -2502,7 +2502,7 @@
         <v>460</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -2520,7 +2520,7 @@
         <v>542</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>563</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>560</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>664</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2588,7 +2588,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>691</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2622,7 +2622,7 @@
         <v>618</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>692</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>555</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,7 +2690,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>460</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>542</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2741,7 +2741,7 @@
         <v>563</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
         <v>618</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2792,7 +2792,7 @@
         <v>560</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
         <v>691</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2843,7 +2843,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
         <v>555</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
         <v>664</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2894,7 +2894,7 @@
         <v>692</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated student ID values in degree plan,removed S values for standardization.
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>DegreeID</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Fall 2019</t>
   </si>
   <si>
-    <t>S533726</t>
-  </si>
-  <si>
     <t>F19</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Sai Tejaswini</t>
   </si>
   <si>
-    <t>S533490</t>
-  </si>
-  <si>
     <t>Gadekari</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
   </si>
   <si>
     <t>Su19</t>
-  </si>
-  <si>
-    <t>S533711</t>
   </si>
   <si>
     <t>Fall 2018</t>
@@ -401,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,6 +438,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,51 +752,51 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>58</v>
+      <c r="A2" s="17">
+        <v>533726</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>58</v>
+      <c r="D2" s="17">
+        <v>533726</v>
       </c>
       <c r="E2" s="7">
         <v>919571565</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="17">
+        <v>533490</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>76</v>
+      <c r="D3" s="17">
+        <v>533490</v>
       </c>
       <c r="E3" s="7">
         <v>919568899</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="17">
+        <v>533711</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>82</v>
+      <c r="D4" s="17">
+        <v>533711</v>
       </c>
       <c r="E4" s="7">
         <v>919570594</v>
@@ -819,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -836,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>9</v>
@@ -1187,10 +1179,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -1207,10 +1199,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1794,7 +1786,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,8 +1815,8 @@
       <c r="A2" s="4">
         <v>7250</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>58</v>
+      <c r="B2" s="4">
+        <v>533726</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>42</v>
@@ -1837,8 +1829,8 @@
       <c r="A3" s="4">
         <v>7251</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>58</v>
+      <c r="B3" s="4">
+        <v>533726</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>40</v>
@@ -1851,50 +1843,50 @@
       <c r="A4" s="4">
         <v>7252</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>76</v>
+      <c r="B4" s="4">
+        <v>533490</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>7253</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>76</v>
+      <c r="B5" s="4">
+        <v>533490</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>7254</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>58</v>
+      <c r="B6" s="4">
+        <v>533726</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>7255</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>58</v>
+      <c r="B7" s="4">
+        <v>533726</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>42</v>
@@ -1913,7 +1905,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,14 +1938,14 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="8">
+        <v>533726</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>57</v>
@@ -1963,116 +1955,116 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>58</v>
+      <c r="B3" s="8">
+        <v>533726</v>
       </c>
       <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>58</v>
+      <c r="B4" s="8">
+        <v>533726</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>58</v>
+      <c r="B5" s="8">
+        <v>533726</v>
       </c>
       <c r="C5" s="8">
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>58</v>
+      <c r="B6" s="8">
+        <v>533726</v>
       </c>
       <c r="C6" s="8">
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>76</v>
+      <c r="B7" s="10">
+        <v>533490</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>76</v>
+      <c r="B8" s="10">
+        <v>533490</v>
       </c>
       <c r="C8" s="10">
         <v>2</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>76</v>
+      <c r="B9" s="10">
+        <v>533490</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>57</v>
@@ -2082,116 +2074,116 @@
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>76</v>
+      <c r="B10" s="10">
+        <v>533490</v>
       </c>
       <c r="C10" s="10">
         <v>4</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>76</v>
+      <c r="B11" s="10">
+        <v>533490</v>
       </c>
       <c r="C11" s="10">
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>76</v>
+      <c r="B12" s="10">
+        <v>533490</v>
       </c>
       <c r="C12" s="10">
         <v>6</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>82</v>
+      <c r="B13" s="12">
+        <v>533711</v>
       </c>
       <c r="C13" s="12">
         <v>1</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>82</v>
+      <c r="B14" s="12">
+        <v>533711</v>
       </c>
       <c r="C14" s="12">
         <v>2</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>82</v>
+      <c r="B15" s="12">
+        <v>533711</v>
       </c>
       <c r="C15" s="12">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>82</v>
+      <c r="B16" s="12">
+        <v>533711</v>
       </c>
       <c r="C16" s="12">
         <v>4</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>57</v>
@@ -2201,34 +2193,34 @@
       <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>82</v>
+      <c r="B17" s="12">
+        <v>533711</v>
       </c>
       <c r="C17" s="12">
         <v>5</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>82</v>
+      <c r="B18" s="12">
+        <v>533711</v>
       </c>
       <c r="C18" s="12">
         <v>6</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added string column to every sheet in the excel sheet
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
   <si>
     <t>DegreeID</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>DegreeName</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -387,17 +390,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -412,7 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,12 +442,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -720,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,74 +744,90 @@
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="12">
+      <c r="E1" s="11">
         <v>919</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="F1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>533726</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="3">
         <v>533726</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="3">
         <v>919571565</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="F2" s="3" t="str">
+        <f>" new Student{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;" , "&amp;$E$1&amp;" = " &amp;E2&amp; " }"</f>
+        <v xml:space="preserve"> new Student{StudentID = 533726 , Family = Narne ,Given =Sai Tejaswini Snumber =533726 , 919 = 919571565 }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>533490</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="3">
         <v>533490</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>919568899</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F4" si="0">" new Student{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;" , "&amp;$E$1&amp;" = " &amp;E3&amp; " }"</f>
+        <v xml:space="preserve"> new Student{StudentID = 533490 , Family = Gadekari ,Given =Sonam Snumber =533490 , 919 = 919568899 }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>533711</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="3">
         <v>533711</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="3">
         <v>919570594</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Student{StudentID = 533711 , Family = Naidu ,Given =Harika Snumber =533711 , 919 = 919570594 }</v>
       </c>
     </row>
   </sheetData>
@@ -809,10 +837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,94 +849,114 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="E1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="E2" s="3" t="str">
+        <f>" new Degree{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;"}"</f>
+        <v xml:space="preserve"> new Degree{DegreeID = 1 , DegreeAbbrev = ACS+2 ,DegreeName =MS ACS+2 NumberOfTerms =5}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="E3" s="3" t="str">
+        <f t="shared" ref="E3:E5" si="0">" new Degree{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;"}"</f>
+        <v xml:space="preserve"> new Degree{DegreeID = 2 , DegreeAbbrev = ACS+DB ,DegreeName =MS ACS + DB NumberOfTerms =5}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Degree{DegreeID = 3 , DegreeAbbrev = ACS+NF ,DegreeName =MS ACS + NF NumberOfTerms =5}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Degree{DegreeID = 4 , DegreeAbbrev = ACS ,DegreeName =MS ACS NumberOfTerms =5}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
   </sheetData>
@@ -918,10 +966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,289 +980,345 @@
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="112" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="G1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>460</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f>" new Credit{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;" , "&amp;$E$1&amp;" ="&amp;E2&amp;", "&amp;$F$1&amp;" ="&amp;F2&amp;"}"</f>
+        <v xml:space="preserve"> new Credit{CreditID = 460 , CreditAbbrev = DB ,CreditName =Databases IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>356</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="str">
+        <f t="shared" ref="G3:G14" si="0">" new Credit{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;" , "&amp;$E$1&amp;" ="&amp;E3&amp;", "&amp;$F$1&amp;" ="&amp;F3&amp;"}"</f>
+        <v xml:space="preserve"> new Credit{CreditID = 356 , CreditAbbrev = NF ,CreditName =Network Fundamentals IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>542</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>542</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 542 , CreditAbbrev = 542 ,CreditName =OOP with Java IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>563</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>563</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 563 , CreditAbbrev = 563 ,CreditName =Web Apps IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>560</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>560</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 560 , CreditAbbrev = 560 ,CreditName =Advanced Databases IsSummer =1 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>664</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 664 , CreditAbbrev = 664-UX ,CreditName =User Experience IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>618</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 618 , CreditAbbrev = 618-PM ,CreditName =Project Management IsSummer =1 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>555</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 555 , CreditAbbrev = 555-NS ,CreditName =Network Security IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>691</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 691 , CreditAbbrev = 691-GDP1 ,CreditName =GDP-1 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>692</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 692 , CreditAbbrev = 692-GDP2 ,CreditName =GDP-2 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>0</v>
       </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 6 , CreditAbbrev = Mobile ,CreditName =643 or 644 Mobile IsSummer =0 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 1 , CreditAbbrev = E1 ,CreditName =Elective1 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>2</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Credit{CreditID = 2 , CreditAbbrev = E2 ,CreditName =Elective2 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
   </sheetData>
@@ -1224,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,545 +1339,741 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="D1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="D2" s="4" t="str">
+        <f>" new DegreeCredit{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;"}"</f>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 1 , DegreeID = 1 ,CreditID =460}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="D3" s="4" t="str">
+        <f t="shared" ref="D3:D49" si="0">" new DegreeCredit{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;"}"</f>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 2 , DegreeID = 1 ,CreditID =356}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
         <v>542</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="D4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 3 , DegreeID = 1 ,CreditID =542}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="D5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 4 , DegreeID = 1 ,CreditID =563}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 5 , DegreeID = 1 ,CreditID =560}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
         <v>664</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 6 , DegreeID = 1 ,CreditID =664}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
         <v>618</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 7 , DegreeID = 1 ,CreditID =618}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
         <v>555</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 8 , DegreeID = 1 ,CreditID =555}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 9 , DegreeID = 1 ,CreditID =691}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
         <v>692</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 10 , DegreeID = 1 ,CreditID =692}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 11 , DegreeID = 1 ,CreditID =6}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 12 , DegreeID = 1 ,CreditID =1}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="D14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 13 , DegreeID = 1 ,CreditID =2}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>460</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="D15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 14 , DegreeID = 2 ,CreditID =460}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>542</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="D16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 15 , DegreeID = 2 ,CreditID =542}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="D17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 16 , DegreeID = 2 ,CreditID =563}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>560</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 17 , DegreeID = 2 ,CreditID =560}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>2</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>664</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 18 , DegreeID = 2 ,CreditID =664}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>618</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 19 , DegreeID = 2 ,CreditID =618}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>555</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="D21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 20 , DegreeID = 2 ,CreditID =555}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>2</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="D22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 21 , DegreeID = 2 ,CreditID =691}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>692</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 22 , DegreeID = 2 ,CreditID =692}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="D24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 23 , DegreeID = 2 ,CreditID =6}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>2</v>
       </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 24 , DegreeID = 2 ,CreditID =1}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>2</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="D26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 25 , DegreeID = 2 ,CreditID =2}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>3</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>356</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="D27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 26 , DegreeID = 3 ,CreditID =356}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>3</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>542</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="D28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 27 , DegreeID = 3 ,CreditID =542}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="D29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 28 , DegreeID = 3 ,CreditID =563}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>3</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>560</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="D30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 29 , DegreeID = 3 ,CreditID =560}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>3</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>664</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="D31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 30 , DegreeID = 3 ,CreditID =664}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>3</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>618</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="D32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 31 , DegreeID = 3 ,CreditID =618}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>3</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>555</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="D33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 32 , DegreeID = 3 ,CreditID =555}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>3</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="D34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 33 , DegreeID = 3 ,CreditID =691}</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>3</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>692</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="D35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 34 , DegreeID = 3 ,CreditID =692}</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>3</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="D36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 35 , DegreeID = 3 ,CreditID =6}</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>3</v>
       </c>
-      <c r="C37" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="C37" s="4">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 36 , DegreeID = 3 ,CreditID =1}</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>3</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="D38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 37 , DegreeID = 3 ,CreditID =2}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="4">
         <v>4</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>542</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="D39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 38 , DegreeID = 4 ,CreditID =542}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>4</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="D40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 39 , DegreeID = 4 ,CreditID =563}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="4">
         <v>4</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="4">
         <v>560</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="D41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 40 , DegreeID = 4 ,CreditID =560}</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>4</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>664</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="D42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 41 , DegreeID = 4 ,CreditID =664}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="4">
         <v>4</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>618</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="D43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 42 , DegreeID = 4 ,CreditID =618}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>4</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>555</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="D44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 43 , DegreeID = 4 ,CreditID =555}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="4">
         <v>4</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="D45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 44 , DegreeID = 4 ,CreditID =691}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>4</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>692</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="D46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 45 , DegreeID = 4 ,CreditID =692}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="4">
         <v>4</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="D47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 46 , DegreeID = 4 ,CreditID =6}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>4</v>
       </c>
-      <c r="C48" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 47 , DegreeID = 4 ,CreditID =1}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="4">
         <v>4</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="4">
         <v>2</v>
+      </c>
+      <c r="D49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 48 , DegreeID = 4 ,CreditID =2}</v>
       </c>
     </row>
   </sheetData>
@@ -1783,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,105 +2094,134 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="147.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="E1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>7250</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>533726</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="E2" s="3" t="str">
+        <f>" new DegreePlan{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;"}"</f>
+        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7250 , StudentID = 533726 ,DegreePlanAbbrev =Slow and Easy DegreePlanName =Take a Summer off}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>7251</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>533726</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="E3" s="3" t="str">
+        <f t="shared" ref="E3:E7" si="0">" new DegreePlan{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;"}"</f>
+        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7251 , StudentID = 533726 ,DegreePlanAbbrev =Super Fast DegreePlanName =As fast as I can}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>7252</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>533490</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7252 , StudentID = 533490 ,DegreePlanAbbrev =Spring Super Slow DegreePlanName =As slow as it could be
+ with a Summer off}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>7253</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>533490</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="E5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7253 , StudentID = 533490 ,DegreePlanAbbrev =Spring Super fast DegreePlanName =As fast as it could be}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>7254</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>533711</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="E6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7254 , StudentID = 533711 ,DegreePlanAbbrev =Early completion DegreePlanName =Fall 2018 fast track}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>7255</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>533711</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>43</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7255 , StudentID = 533711 ,DegreePlanAbbrev =Slow and Easy DegreePlanName =Take a Summer off}</v>
       </c>
     </row>
   </sheetData>
@@ -1902,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,313 +2243,385 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="107.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
+      <c r="F1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13">
         <v>533726</v>
       </c>
-      <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="F2" s="14" t="str">
+        <f>" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;" ,  "&amp;$E$1&amp;" ="&amp;E2&amp;"}"</f>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 1 , StudentID = 533726 ,Term =1 TermAbbrev =F19 ,  TermName =Fall 2019}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="13">
         <v>533726</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="13">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="F3" s="14" t="str">
+        <f t="shared" ref="F3:F18" si="0">" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;" ,  "&amp;$E$1&amp;" ="&amp;E3&amp;"}"</f>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 2 , StudentID = 533726 ,Term =2 TermAbbrev =S20 ,  TermName =Spring 2020}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <v>533726</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="13">
         <v>3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="F4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 3 , StudentID = 533726 ,Term =3 TermAbbrev =Su20 ,  TermName =Summer 2020}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="13">
         <v>533726</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>4</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="F5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 4 , StudentID = 533726 ,Term =4 TermAbbrev =F20 ,  TermName =Fall 2020}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="13">
         <v>533726</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>5</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="F6" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 5 , StudentID = 533726 ,Term =5 TermAbbrev =S21 ,  TermName =Spring 2021}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>533490</v>
       </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="F7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 6 , StudentID = 533490 ,Term =1 TermAbbrev =S19 ,  TermName =Spring 2019}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>533490</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>2</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="F8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 7 , StudentID = 533490 ,Term =2 TermAbbrev =Su19 ,  TermName =Summer 2019}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>533490</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="F9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 8 , StudentID = 533490 ,Term =3 TermAbbrev =F19 ,  TermName =Fall 2019}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>533490</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="F10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 9 , StudentID = 533490 ,Term =4 TermAbbrev =S20 ,  TermName =Spring 2020}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>533490</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="F11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 10 , StudentID = 533490 ,Term =5 TermAbbrev =Su20 ,  TermName =Summer 2020}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>533490</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>6</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="F12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 11 , StudentID = 533490 ,Term =6 TermAbbrev =F20 ,  TermName =Fall 2020}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="8">
         <v>533711</v>
       </c>
-      <c r="C13" s="10">
-        <v>1</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="F13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 12 , StudentID = 533711 ,Term =1 TermAbbrev =F18 ,  TermName =Fall 2018}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="8">
         <v>533711</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <v>2</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="F14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 13 , StudentID = 533711 ,Term =2 TermAbbrev =S19 ,  TermName =Spring 2019}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="8">
         <v>533711</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <v>3</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="F15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 14 , StudentID = 533711 ,Term =3 TermAbbrev =Su19 ,  TermName =Summer 2019}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="8">
         <v>533711</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>4</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="F16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 15 , StudentID = 533711 ,Term =4 TermAbbrev =F19 ,  TermName =Fall 2019}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="8">
         <v>533711</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>5</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="F17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 16 , StudentID = 533711 ,Term =5 TermAbbrev =S20 ,  TermName =Spring 2020}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="8">
         <v>533711</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>6</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="9" t="s">
         <v>65</v>
+      </c>
+      <c r="F18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 17 , StudentID = 533711 ,Term =6 TermAbbrev =Su19 ,  TermName =Summer 2020}</v>
       </c>
     </row>
   </sheetData>
@@ -2233,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,650 +2644,783 @@
     <col min="3" max="3" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>7251</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>460</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="3" t="str">
+        <f>" new Slot{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;", "&amp;$E$1&amp;" ="&amp;E2&amp;"}"</f>
+        <v xml:space="preserve"> new Slot{SlotID = 1 , DegreePlan = 7251 ,Term =1 CreditID =460, Status =C}</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>7251</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
         <v>542</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F37" si="0">" new Slot{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;", "&amp;$E$1&amp;" ="&amp;E3&amp;"}"</f>
+        <v xml:space="preserve"> new Slot{SlotID = 2 , DegreePlan = 7251 ,Term =1 CreditID =542, Status =C}</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>7251</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>563</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 3 , DegreePlan = 7251 ,Term =1 CreditID =563, Status =C}</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>7251</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>560</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 4 , DegreePlan = 7251 ,Term =2 CreditID =560, Status =A}</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>7251</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>664</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 5 , DegreePlan = 7251 ,Term =2 CreditID =664, Status =A}</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>7251</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 6 , DegreePlan = 7251 ,Term =2 CreditID =6, Status =A}</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>7251</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>618</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 7 , DegreePlan = 7251 ,Term =3 CreditID =618, Status =P}</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>7251</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>691</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 8 , DegreePlan = 7251 ,Term =3 CreditID =691, Status =P}</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>7251</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>692</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 9 , DegreePlan = 7251 ,Term =4 CreditID =692, Status =P}</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>7251</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 10 , DegreePlan = 7251 ,Term =4 CreditID =1, Status =P}</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>7251</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>4</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 11 , DegreePlan = 7251 ,Term =4 CreditID =2, Status =P}</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>7251</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>5</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>555</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 12 , DegreePlan = 7251 ,Term =5 CreditID =555, Status =P}</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>7252</v>
       </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
         <v>460</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 13 , DegreePlan = 7252 ,Term =1 CreditID =460, Status =C}</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>7252</v>
       </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
         <v>542</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="F15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 14 , DegreePlan = 7252 ,Term =1 CreditID =542, Status =C}</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>7252</v>
       </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
         <v>563</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="F16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 15 , DegreePlan = 7252 ,Term =1 CreditID =563, Status =C}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>7252</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>560</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="F17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 16 , DegreePlan = 7252 ,Term =3 CreditID =560, Status =C}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>7252</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>3</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>664</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="F18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 17 , DegreePlan = 7252 ,Term =3 CreditID =664, Status =A}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>7252</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>6</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="F19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 18 , DegreePlan = 7252 ,Term =3 CreditID =6, Status =A}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>7252</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>4</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>691</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="F20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 19 , DegreePlan = 7252 ,Term =4 CreditID =691, Status =A}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>7252</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>4</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>618</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="F21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 20 , DegreePlan = 7252 ,Term =4 CreditID =618, Status =P}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>7252</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>5</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>692</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="F22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 21 , DegreePlan = 7252 ,Term =5 CreditID =692, Status =P}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>7252</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>5</v>
       </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="F23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 22 , DegreePlan = 7252 ,Term =5 CreditID =1, Status =P}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>7252</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>6</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>555</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 23 , DegreePlan = 7252 ,Term =6 CreditID =555, Status =P}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>7252</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>6</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 24 , DegreePlan = 7252 ,Term =6 CreditID =2, Status =P}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>7255</v>
       </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4">
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
         <v>460</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="F26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 25 , DegreePlan = 7255 ,Term =1 CreditID =460, Status =C}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>7255</v>
       </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4">
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
         <v>542</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="F27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 26 , DegreePlan = 7255 ,Term =1 CreditID =542, Status =C}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>7255</v>
       </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4">
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
         <v>563</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="F28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 27 , DegreePlan = 7255 ,Term =1 CreditID =563, Status =C}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>7255</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>2</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>6</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="F29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 28 , DegreePlan = 7255 ,Term =2 CreditID =6, Status =A}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>7255</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>2</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>618</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 29 , DegreePlan = 7255 ,Term =2 CreditID =618, Status =A}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>7255</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>2</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>560</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 30 , DegreePlan = 7255 ,Term =2 CreditID =560, Status =A}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>7255</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>4</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>691</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 31 , DegreePlan = 7255 ,Term =4 CreditID =691, Status =P}</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>7255</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>4</v>
       </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="F33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 32 , DegreePlan = 7255 ,Term =4 CreditID =1, Status =P}</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>7255</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>4</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>2</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="F34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 33 , DegreePlan = 7255 ,Term =4 CreditID =2, Status =P}</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>7255</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>5</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>555</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="F35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 34 , DegreePlan = 7255 ,Term =5 CreditID =555, Status =P}</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>7255</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>5</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>664</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="F36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 35 , DegreePlan = 7255 ,Term =5 CreditID =664, Status =P}</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>7255</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>6</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>692</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="F37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot{SlotID = 36 , DegreePlan = 7255 ,Term =6 CreditID =692, Status =P}</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit to DBContext file
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533726\Desktop\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533490\Documents\44663\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
   <si>
     <t>DegreeID</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>new Degree{DegreeID = 1, DegreeAbbrev = "ACS+2", DegreeName ="MS ACS+2", NumberOfTerms = 5}</t>
+  </si>
+  <si>
+    <t>new Degree{DegreeID = 2, DegreeAbbrev = "ACS+DB", DegreeName ="MS ACS + DB", NumberOfTerms = 5}</t>
+  </si>
+  <si>
+    <t>new Degree{DegreeID = 3, DegreeAbbrev = "ACS+NF", DegreeName ="MS ACS + NF", NumberOfTerms = 5}</t>
+  </si>
+  <si>
+    <t>new Degree{DegreeID = 4, DegreeAbbrev = "ACS", DegreeName ="MS ACS", NumberOfTerms = 5}</t>
   </si>
 </sst>
 </file>
@@ -839,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,9 +894,8 @@
       <c r="D2" s="3">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="str">
-        <f>" new Degree{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;"}"</f>
-        <v xml:space="preserve"> new Degree{DegreeID = 1 , DegreeAbbrev = ACS+2 ,DegreeName =MS ACS+2 NumberOfTerms =5}</v>
+      <c r="E2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -900,9 +911,8 @@
       <c r="D3" s="3">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E5" si="0">" new Degree{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;"}"</f>
-        <v xml:space="preserve"> new Degree{DegreeID = 2 , DegreeAbbrev = ACS+DB ,DegreeName =MS ACS + DB NumberOfTerms =5}</v>
+      <c r="E3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,9 +928,8 @@
       <c r="D4" s="3">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Degree{DegreeID = 3 , DegreeAbbrev = ACS+NF ,DegreeName =MS ACS + NF NumberOfTerms =5}</v>
+      <c r="E4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -936,9 +945,8 @@
       <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Degree{DegreeID = 4 , DegreeAbbrev = ACS ,DegreeName =MS ACS NumberOfTerms =5}</v>
+      <c r="E5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,7 +2642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DbInitializer.cs is added ,ApplicationDbContext.cs
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
   <si>
     <t>DegreeID</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>new Degree{DegreeID = 4, DegreeAbbrev = "ACS", DegreeName ="MS ACS", NumberOfTerms = 5}</t>
+  </si>
+  <si>
+    <t>number_919</t>
   </si>
 </sst>
 </file>
@@ -746,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +759,7 @@
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,8 +775,8 @@
       <c r="D1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="11">
-        <v>919</v>
+      <c r="E1" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>91</v>
@@ -796,8 +799,8 @@
         <v>919571565</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>" new Student{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;" , "&amp;$E$1&amp;" = " &amp;E2&amp; " }"</f>
-        <v xml:space="preserve"> new Student{StudentID = 533726 , Family = Narne ,Given =Sai Tejaswini Snumber =533726 , 919 = 919571565 }</v>
+        <f>CONCATENATE("new Student{StudentID = ",A:A," , Family = ''",B:B,"'' , Given =''",C:C,"''",", Snumber =",D:D," , number_919=",E:E,"}")</f>
+        <v>new Student{StudentID = 533726 , Family = ''Narne'' , Given =''Sai Tejaswini'', Snumber =533726 , number_919=919571565}</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -817,8 +820,8 @@
         <v>919568899</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F4" si="0">" new Student{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;" , "&amp;$E$1&amp;" = " &amp;E3&amp; " }"</f>
-        <v xml:space="preserve"> new Student{StudentID = 533490 , Family = Gadekari ,Given =Sonam Snumber =533490 , 919 = 919568899 }</v>
+        <f t="shared" ref="F3:F4" si="0">CONCATENATE("new Student{StudentID = ",A:A," , Family = ''",B:B,"'' , Given =''",C:C,"''",", Snumber =",D:D," , number_919=",E:E,"}")</f>
+        <v>new Student{StudentID = 533490 , Family = ''Gadekari'' , Given =''Sonam'', Snumber =533490 , number_919=919568899}</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,7 +842,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Student{StudentID = 533711 , Family = Naidu ,Given =Harika Snumber =533711 , 919 = 919570594 }</v>
+        <v>new Student{StudentID = 533711 , Family = ''Naidu'' , Given =''Harika'', Snumber =533711 , number_919=919570594}</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
commit the changes in DegreePlan.cs and seeding the data in DbInitializer.cs i.e added the Credit and DegreePlan
Changes also done in the worksheet i.e added string for DegreePlan and Credit sheets
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533490\Documents\44663\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533726\Desktop\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -290,10 +290,6 @@
     <t>As fast as it could be</t>
   </si>
   <si>
-    <t>As slow as it could be
- with a Summer off</t>
-  </si>
-  <si>
     <t>Early completion</t>
   </si>
   <si>
@@ -322,6 +318,9 @@
   </si>
   <si>
     <t>number_919</t>
+  </si>
+  <si>
+    <t>As slow as it could be with a Summer off</t>
   </si>
 </sst>
 </file>
@@ -749,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -776,10 +775,10 @@
         <v>46</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,7 +854,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,16 +871,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,7 +914,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,7 +931,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -980,7 +979,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +990,7 @@
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="112" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="118.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1014,7 +1013,7 @@
         <v>34</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1037,8 +1036,8 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="str">
-        <f>" new Credit{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;" , "&amp;$E$1&amp;" ="&amp;E2&amp;", "&amp;$F$1&amp;" ="&amp;F2&amp;"}"</f>
-        <v xml:space="preserve"> new Credit{CreditID = 460 , CreditAbbrev = DB ,CreditName =Databases IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <f t="shared" ref="G2:G14" si="0">CONCATENATE("new Credit{CreditID = ",A:A," , CreditAbbrev = ''",B:B,"'' ,CreditName = ''",C:C,"'', IsSummer = ",D:D," , IsSpring = ",E:E,", IsFall = ",F:F,"},")</f>
+        <v>new Credit{CreditID = 460 , CreditAbbrev = ''DB'' ,CreditName = ''Databases'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,8 +1060,8 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="str">
-        <f t="shared" ref="G3:G14" si="0">" new Credit{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;" , "&amp;$E$1&amp;" ="&amp;E3&amp;", "&amp;$F$1&amp;" ="&amp;F3&amp;"}"</f>
-        <v xml:space="preserve"> new Credit{CreditID = 356 , CreditAbbrev = NF ,CreditName =Network Fundamentals IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <f t="shared" si="0"/>
+        <v>new Credit{CreditID = 356 , CreditAbbrev = ''NF'' ,CreditName = ''Network Fundamentals'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1086,7 +1085,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 542 , CreditAbbrev = 542 ,CreditName =OOP with Java IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 542 , CreditAbbrev = ''542'' ,CreditName = ''OOP with Java'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1110,7 +1109,7 @@
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 563 , CreditAbbrev = 563 ,CreditName =Web Apps IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 563 , CreditAbbrev = ''563'' ,CreditName = ''Web Apps'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1134,7 +1133,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 560 , CreditAbbrev = 560 ,CreditName =Advanced Databases IsSummer =1 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 560 , CreditAbbrev = ''560'' ,CreditName = ''Advanced Databases'', IsSummer = 1 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1158,7 +1157,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 664 , CreditAbbrev = 664-UX ,CreditName =User Experience IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 664 , CreditAbbrev = ''664-UX'' ,CreditName = ''User Experience'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,7 +1181,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 618 , CreditAbbrev = 618-PM ,CreditName =Project Management IsSummer =1 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 618 , CreditAbbrev = ''618-PM'' ,CreditName = ''Project Management'', IsSummer = 1 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1206,7 +1205,7 @@
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 555 , CreditAbbrev = 555-NS ,CreditName =Network Security IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 555 , CreditAbbrev = ''555-NS'' ,CreditName = ''Network Security'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1230,7 +1229,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 691 , CreditAbbrev = 691-GDP1 ,CreditName =GDP-1 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 691 , CreditAbbrev = ''691-GDP1'' ,CreditName = ''GDP-1'', IsSummer = 1 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1254,7 +1253,7 @@
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 692 , CreditAbbrev = 692-GDP2 ,CreditName =GDP-2 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 692 , CreditAbbrev = ''692-GDP2'' ,CreditName = ''GDP-2'', IsSummer = 1 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1278,7 +1277,7 @@
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 6 , CreditAbbrev = Mobile ,CreditName =643 or 644 Mobile IsSummer =0 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 6 , CreditAbbrev = ''Mobile'' ,CreditName = ''643 or 644 Mobile'', IsSummer = 0 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1302,7 +1301,7 @@
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 1 , CreditAbbrev = E1 ,CreditName =Elective1 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 1 , CreditAbbrev = ''E1'' ,CreditName = ''Elective1'', IsSummer = 1 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1326,7 +1325,7 @@
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{CreditID = 2 , CreditAbbrev = E2 ,CreditName =Elective2 IsSummer =1 , IsSpring =1, IsFall =1}</v>
+        <v>new Credit{CreditID = 2 , CreditAbbrev = ''E2'' ,CreditName = ''Elective2'', IsSummer = 1 , IsSpring = 1, IsFall = 1},</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1364,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,8 +2104,8 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="147.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="150.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2123,7 +2122,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,8 +2139,8 @@
         <v>43</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>" new DegreePlan{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;"}"</f>
-        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7250 , StudentID = 533726 ,DegreePlanAbbrev =Slow and Easy DegreePlanName =Take a Summer off}</v>
+        <f>CONCATENATE("new DegreePlan{DegreePlanID = ",A:A," , StudentID = ",B:B," ,DegreePlanAbbrev = ''",C:C,"'', DegreePlanName =''",D:D,"''}")</f>
+        <v>new DegreePlan{DegreePlanID = 7250 , StudentID = 533726 ,DegreePlanAbbrev = ''Slow and Easy'', DegreePlanName =''Take a Summer off''}</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2158,11 +2157,11 @@
         <v>41</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E7" si="0">" new DegreePlan{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;"}"</f>
-        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7251 , StudentID = 533726 ,DegreePlanAbbrev =Super Fast DegreePlanName =As fast as I can}</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E3:E7" si="0">CONCATENATE("new DegreePlan{DegreePlanID = ",A:A," , StudentID = ",B:B," ,DegreePlanAbbrev = ''",C:C,"'', DegreePlanName =''",D:D,"''}")</f>
+        <v>new DegreePlan{DegreePlanID = 7251 , StudentID = 533726 ,DegreePlanAbbrev = ''Super Fast'', DegreePlanName =''As fast as I can''}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>7252</v>
       </c>
@@ -2173,12 +2172,11 @@
         <v>83</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7252 , StudentID = 533490 ,DegreePlanAbbrev =Spring Super Slow DegreePlanName =As slow as it could be
- with a Summer off}</v>
+        <v>new DegreePlan{DegreePlanID = 7252 , StudentID = 533490 ,DegreePlanAbbrev = ''Spring Super Slow'', DegreePlanName =''As slow as it could be with a Summer off''}</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2196,7 +2194,7 @@
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7253 , StudentID = 533490 ,DegreePlanAbbrev =Spring Super fast DegreePlanName =As fast as it could be}</v>
+        <v>new DegreePlan{DegreePlanID = 7253 , StudentID = 533490 ,DegreePlanAbbrev = ''Spring Super fast'', DegreePlanName =''As fast as it could be''}</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2207,14 +2205,14 @@
         <v>533711</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7254 , StudentID = 533711 ,DegreePlanAbbrev =Early completion DegreePlanName =Fall 2018 fast track}</v>
+        <v>new DegreePlan{DegreePlanID = 7254 , StudentID = 533711 ,DegreePlanAbbrev = ''Early completion'', DegreePlanName =''Fall 2018 fast track''}</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2232,7 +2230,7 @@
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreePlan{DegreePlanID = 7255 , StudentID = 533711 ,DegreePlanAbbrev =Slow and Easy DegreePlanName =Take a Summer off}</v>
+        <v>new DegreePlan{DegreePlanID = 7255 , StudentID = 533711 ,DegreePlanAbbrev = ''Slow and Easy'', DegreePlanName =''Take a Summer off''}</v>
       </c>
     </row>
   </sheetData>
@@ -2244,7 +2242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2275,7 +2273,7 @@
         <v>56</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,7 +2673,7 @@
         <v>48</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added DbInitializer.cs with my Issues Assigned
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533726\Desktop\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533711\Desktop\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,8 +798,8 @@
         <v>919571565</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>CONCATENATE("new Student{StudentID = ",A:A," , Family = ''",B:B,"'' , Given =''",C:C,"''",", Snumber =",D:D," , number_919=",E:E,"}")</f>
-        <v>new Student{StudentID = 533726 , Family = ''Narne'' , Given =''Sai Tejaswini'', Snumber =533726 , number_919=919571565}</v>
+        <f>CONCATENATE("new Student{StudentID = ",A:A," , Family = ''",B:B,"'' , Given =''",C:C,"''",", Snumber =",D:D," , number_919=",E:E,"},")</f>
+        <v>new Student{StudentID = 533726 , Family = ''Narne'' , Given =''Sai Tejaswini'', Snumber =533726 , number_919=919571565},</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,8 +819,8 @@
         <v>919568899</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F4" si="0">CONCATENATE("new Student{StudentID = ",A:A," , Family = ''",B:B,"'' , Given =''",C:C,"''",", Snumber =",D:D," , number_919=",E:E,"}")</f>
-        <v>new Student{StudentID = 533490 , Family = ''Gadekari'' , Given =''Sonam'', Snumber =533490 , number_919=919568899}</v>
+        <f t="shared" ref="F3:F4" si="0">CONCATENATE("new Student{StudentID = ",A:A," , Family = ''",B:B,"'' , Given =''",C:C,"''",", Snumber =",D:D," , number_919=",E:E,"},")</f>
+        <v>new Student{StudentID = 533490 , Family = ''Gadekari'' , Given =''Sonam'', Snumber =533490 , number_919=919568899},</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Student{StudentID = 533711 , Family = ''Naidu'' , Given =''Harika'', Snumber =533711 , number_919=919570594}</v>
+        <v>new Student{StudentID = 533711 , Family = ''Naidu'' , Given =''Harika'', Snumber =533711 , number_919=919570594},</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D2" sqref="D2:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,8 +1377,8 @@
         <v>460</v>
       </c>
       <c r="D2" s="4" t="str">
-        <f>" new DegreeCredit{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;"}"</f>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 1 , DegreeID = 1 ,CreditID =460}</v>
+        <f>" new DegreeCredit{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;"},"</f>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 1 , DegreeID = 1 ,CreditID =460},</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,8 +1392,8 @@
         <v>356</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D49" si="0">" new DegreeCredit{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;"}"</f>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 2 , DegreeID = 1 ,CreditID =356}</v>
+        <f t="shared" ref="D3:D49" si="0">" new DegreeCredit{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;"},"</f>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 2 , DegreeID = 1 ,CreditID =356},</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 3 , DegreeID = 1 ,CreditID =542}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 3 , DegreeID = 1 ,CreditID =542},</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 4 , DegreeID = 1 ,CreditID =563}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 4 , DegreeID = 1 ,CreditID =563},</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 5 , DegreeID = 1 ,CreditID =560}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 5 , DegreeID = 1 ,CreditID =560},</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 6 , DegreeID = 1 ,CreditID =664}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 6 , DegreeID = 1 ,CreditID =664},</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 7 , DegreeID = 1 ,CreditID =618}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 7 , DegreeID = 1 ,CreditID =618},</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 8 , DegreeID = 1 ,CreditID =555}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 8 , DegreeID = 1 ,CreditID =555},</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1498,7 +1498,7 @@
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 9 , DegreeID = 1 ,CreditID =691}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 9 , DegreeID = 1 ,CreditID =691},</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 10 , DegreeID = 1 ,CreditID =692}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 10 , DegreeID = 1 ,CreditID =692},</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 11 , DegreeID = 1 ,CreditID =6}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 11 , DegreeID = 1 ,CreditID =6},</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 12 , DegreeID = 1 ,CreditID =1}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 12 , DegreeID = 1 ,CreditID =1},</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 13 , DegreeID = 1 ,CreditID =2}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 13 , DegreeID = 1 ,CreditID =2},</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 14 , DegreeID = 2 ,CreditID =460}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 14 , DegreeID = 2 ,CreditID =460},</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="D16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 15 , DegreeID = 2 ,CreditID =542}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 15 , DegreeID = 2 ,CreditID =542},</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 16 , DegreeID = 2 ,CreditID =563}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 16 , DegreeID = 2 ,CreditID =563},</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 17 , DegreeID = 2 ,CreditID =560}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 17 , DegreeID = 2 ,CreditID =560},</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 18 , DegreeID = 2 ,CreditID =664}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 18 , DegreeID = 2 ,CreditID =664},</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="D20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 19 , DegreeID = 2 ,CreditID =618}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 19 , DegreeID = 2 ,CreditID =618},</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="D21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 20 , DegreeID = 2 ,CreditID =555}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 20 , DegreeID = 2 ,CreditID =555},</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="D22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 21 , DegreeID = 2 ,CreditID =691}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 21 , DegreeID = 2 ,CreditID =691},</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 22 , DegreeID = 2 ,CreditID =692}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 22 , DegreeID = 2 ,CreditID =692},</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="D24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 23 , DegreeID = 2 ,CreditID =6}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 23 , DegreeID = 2 ,CreditID =6},</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="D25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 24 , DegreeID = 2 ,CreditID =1}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 24 , DegreeID = 2 ,CreditID =1},</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="D26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 25 , DegreeID = 2 ,CreditID =2}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 25 , DegreeID = 2 ,CreditID =2},</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 26 , DegreeID = 3 ,CreditID =356}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 26 , DegreeID = 3 ,CreditID =356},</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 27 , DegreeID = 3 ,CreditID =542}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 27 , DegreeID = 3 ,CreditID =542},</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="D29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 28 , DegreeID = 3 ,CreditID =563}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 28 , DegreeID = 3 ,CreditID =563},</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="D30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 29 , DegreeID = 3 ,CreditID =560}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 29 , DegreeID = 3 ,CreditID =560},</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="D31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 30 , DegreeID = 3 ,CreditID =664}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 30 , DegreeID = 3 ,CreditID =664},</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="D32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 31 , DegreeID = 3 ,CreditID =618}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 31 , DegreeID = 3 ,CreditID =618},</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="D33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 32 , DegreeID = 3 ,CreditID =555}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 32 , DegreeID = 3 ,CreditID =555},</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="D34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 33 , DegreeID = 3 ,CreditID =691}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 33 , DegreeID = 3 ,CreditID =691},</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="D35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 34 , DegreeID = 3 ,CreditID =692}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 34 , DegreeID = 3 ,CreditID =692},</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="D36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 35 , DegreeID = 3 ,CreditID =6}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 35 , DegreeID = 3 ,CreditID =6},</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 36 , DegreeID = 3 ,CreditID =1}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 36 , DegreeID = 3 ,CreditID =1},</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="D38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 37 , DegreeID = 3 ,CreditID =2}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 37 , DegreeID = 3 ,CreditID =2},</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="D39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 38 , DegreeID = 4 ,CreditID =542}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 38 , DegreeID = 4 ,CreditID =542},</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="D40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 39 , DegreeID = 4 ,CreditID =563}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 39 , DegreeID = 4 ,CreditID =563},</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="D41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 40 , DegreeID = 4 ,CreditID =560}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 40 , DegreeID = 4 ,CreditID =560},</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="D42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 41 , DegreeID = 4 ,CreditID =664}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 41 , DegreeID = 4 ,CreditID =664},</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="D43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 42 , DegreeID = 4 ,CreditID =618}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 42 , DegreeID = 4 ,CreditID =618},</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="D44" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 43 , DegreeID = 4 ,CreditID =555}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 43 , DegreeID = 4 ,CreditID =555},</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D45" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 44 , DegreeID = 4 ,CreditID =691}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 44 , DegreeID = 4 ,CreditID =691},</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="D46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 45 , DegreeID = 4 ,CreditID =692}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 45 , DegreeID = 4 ,CreditID =692},</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="D47" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 46 , DegreeID = 4 ,CreditID =6}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 46 , DegreeID = 4 ,CreditID =6},</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="D48" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 47 , DegreeID = 4 ,CreditID =1}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 47 , DegreeID = 4 ,CreditID =1},</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="D49" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 48 , DegreeID = 4 ,CreditID =2}</v>
+        <v xml:space="preserve"> new DegreeCredit{DegreeCreditID = 48 , DegreeID = 4 ,CreditID =2},</v>
       </c>
     </row>
   </sheetData>
@@ -2095,7 +2095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Models StudentTerm.cs and Slot.cs are updated. Seeded the data into StudentTerm and Slot tables
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533711\Desktop\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533490\Documents\44663\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -420,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,6 +465,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +855,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +880,7 @@
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>90</v>
       </c>
     </row>
@@ -896,7 +897,7 @@
       <c r="D2" s="3">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="16" t="s">
         <v>91</v>
       </c>
     </row>
@@ -913,7 +914,7 @@
       <c r="D3" s="3">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="16" t="s">
         <v>92</v>
       </c>
     </row>
@@ -930,7 +931,7 @@
       <c r="D4" s="3">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
         <v>93</v>
       </c>
     </row>
@@ -947,7 +948,7 @@
       <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="16" t="s">
         <v>94</v>
       </c>
     </row>
@@ -979,7 +980,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2097,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2254,7 @@
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="107.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2293,8 +2294,8 @@
         <v>57</v>
       </c>
       <c r="F2" s="14" t="str">
-        <f>" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;" ,  "&amp;$E$1&amp;" ="&amp;E2&amp;"}"</f>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 1 , StudentID = 533726 ,Term =1 TermAbbrev =F19 ,  TermName =Fall 2019}</v>
+        <f>" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;", "&amp;$D$1&amp;" = ''"&amp;D2&amp;"'',  "&amp;$E$1&amp;" =''"&amp;E2&amp;"'' },"</f>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 1 , StudentID = 533726 ,Term =1, TermAbbrev = ''F19'',  TermName =''Fall 2019'' },</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,8 +2315,8 @@
         <v>66</v>
       </c>
       <c r="F3" s="14" t="str">
-        <f t="shared" ref="F3:F18" si="0">" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;" ,  "&amp;$E$1&amp;" ="&amp;E3&amp;"}"</f>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 2 , StudentID = 533726 ,Term =2 TermAbbrev =S20 ,  TermName =Spring 2020}</v>
+        <f t="shared" ref="F3:F18" si="0">" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;", "&amp;$D$1&amp;" = ''"&amp;D3&amp;"'',  "&amp;$E$1&amp;" =''"&amp;E3&amp;"'' },"</f>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 2 , StudentID = 533726 ,Term =2, TermAbbrev = ''S20'',  TermName =''Spring 2020'' },</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2336,7 +2337,7 @@
       </c>
       <c r="F4" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 3 , StudentID = 533726 ,Term =3 TermAbbrev =Su20 ,  TermName =Summer 2020}</v>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 3 , StudentID = 533726 ,Term =3, TermAbbrev = ''Su20'',  TermName =''Summer 2020'' },</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2357,7 +2358,7 @@
       </c>
       <c r="F5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 4 , StudentID = 533726 ,Term =4 TermAbbrev =F20 ,  TermName =Fall 2020}</v>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 4 , StudentID = 533726 ,Term =4, TermAbbrev = ''F20'',  TermName =''Fall 2020'' },</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2378,7 +2379,7 @@
       </c>
       <c r="F6" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 5 , StudentID = 533726 ,Term =5 TermAbbrev =S21 ,  TermName =Spring 2021}</v>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 5 , StudentID = 533726 ,Term =5, TermAbbrev = ''S21'',  TermName =''Spring 2021'' },</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,9 +2398,9 @@
       <c r="E7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 6 , StudentID = 533490 ,Term =1 TermAbbrev =S19 ,  TermName =Spring 2019}</v>
+      <c r="F7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 6 , StudentID = 533490 ,Term =1, TermAbbrev = ''S19'',  TermName =''Spring 2019'' },</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2418,9 +2419,9 @@
       <c r="E8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 7 , StudentID = 533490 ,Term =2 TermAbbrev =Su19 ,  TermName =Summer 2019}</v>
+      <c r="F8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 7 , StudentID = 533490 ,Term =2, TermAbbrev = ''Su19'',  TermName =''Summer 2019'' },</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,9 +2440,9 @@
       <c r="E9" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 8 , StudentID = 533490 ,Term =3 TermAbbrev =F19 ,  TermName =Fall 2019}</v>
+      <c r="F9" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 8 , StudentID = 533490 ,Term =3, TermAbbrev = ''F19'',  TermName =''Fall 2019'' },</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2460,9 +2461,9 @@
       <c r="E10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 9 , StudentID = 533490 ,Term =4 TermAbbrev =S20 ,  TermName =Spring 2020}</v>
+      <c r="F10" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 9 , StudentID = 533490 ,Term =4, TermAbbrev = ''S20'',  TermName =''Spring 2020'' },</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,9 +2482,9 @@
       <c r="E11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 10 , StudentID = 533490 ,Term =5 TermAbbrev =Su20 ,  TermName =Summer 2020}</v>
+      <c r="F11" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 10 , StudentID = 533490 ,Term =5, TermAbbrev = ''Su20'',  TermName =''Summer 2020'' },</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,9 +2503,9 @@
       <c r="E12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 11 , StudentID = 533490 ,Term =6 TermAbbrev =F20 ,  TermName =Fall 2020}</v>
+      <c r="F12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 11 , StudentID = 533490 ,Term =6, TermAbbrev = ''F20'',  TermName =''Fall 2020'' },</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,9 +2524,9 @@
       <c r="E13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 12 , StudentID = 533711 ,Term =1 TermAbbrev =F18 ,  TermName =Fall 2018}</v>
+      <c r="F13" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 12 , StudentID = 533711 ,Term =1, TermAbbrev = ''F18'',  TermName =''Fall 2018'' },</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,9 +2545,9 @@
       <c r="E14" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 13 , StudentID = 533711 ,Term =2 TermAbbrev =S19 ,  TermName =Spring 2019}</v>
+      <c r="F14" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 13 , StudentID = 533711 ,Term =2, TermAbbrev = ''S19'',  TermName =''Spring 2019'' },</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,9 +2566,9 @@
       <c r="E15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 14 , StudentID = 533711 ,Term =3 TermAbbrev =Su19 ,  TermName =Summer 2019}</v>
+      <c r="F15" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 14 , StudentID = 533711 ,Term =3, TermAbbrev = ''Su19'',  TermName =''Summer 2019'' },</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,9 +2587,9 @@
       <c r="E16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 15 , StudentID = 533711 ,Term =4 TermAbbrev =F19 ,  TermName =Fall 2019}</v>
+      <c r="F16" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 15 , StudentID = 533711 ,Term =4, TermAbbrev = ''F19'',  TermName =''Fall 2019'' },</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,9 +2608,9 @@
       <c r="E17" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 16 , StudentID = 533711 ,Term =5 TermAbbrev =S20 ,  TermName =Spring 2020}</v>
+      <c r="F17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 16 , StudentID = 533711 ,Term =5, TermAbbrev = ''S20'',  TermName =''Spring 2020'' },</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,9 +2629,9 @@
       <c r="E18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new StudentTerm{StudentTermID = 17 , StudentID = 533711 ,Term =6 TermAbbrev =Su19 ,  TermName =Summer 2020}</v>
+      <c r="F18" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new StudentTerm{StudentTermID = 17 , StudentID = 533711 ,Term =6, TermAbbrev = ''Su19'',  TermName =''Summer 2020'' },</v>
       </c>
     </row>
   </sheetData>
@@ -2643,8 +2644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,7 +2654,7 @@
     <col min="3" max="3" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2693,8 +2694,8 @@
         <v>51</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>" new Slot{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" "&amp;$D$1&amp;" ="&amp;D2&amp;", "&amp;$E$1&amp;" ="&amp;E2&amp;"}"</f>
-        <v xml:space="preserve"> new Slot{SlotID = 1 , DegreePlan = 7251 ,Term =1 CreditID =460, Status =C}</v>
+        <f>" new Slot{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;", "&amp;$D$1&amp;" ="&amp;D2&amp;", "&amp;$E$1&amp;" ="&amp;"''"&amp;E2&amp;"'' },"</f>
+        <v xml:space="preserve"> new Slot{SlotID = 1 , DegreePlan = 7251 ,Term =1, CreditID =460, Status =''C'' },</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2714,8 +2715,8 @@
         <v>51</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F37" si="0">" new Slot{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" "&amp;$D$1&amp;" ="&amp;D3&amp;", "&amp;$E$1&amp;" ="&amp;E3&amp;"}"</f>
-        <v xml:space="preserve"> new Slot{SlotID = 2 , DegreePlan = 7251 ,Term =1 CreditID =542, Status =C}</v>
+        <f t="shared" ref="F3:F37" si="0">" new Slot{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;", "&amp;$D$1&amp;" ="&amp;D3&amp;", "&amp;$E$1&amp;" ="&amp;"''"&amp;E3&amp;"'' },"</f>
+        <v xml:space="preserve"> new Slot{SlotID = 2 , DegreePlan = 7251 ,Term =1, CreditID =542, Status =''C'' },</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2736,7 +2737,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 3 , DegreePlan = 7251 ,Term =1 CreditID =563, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 3 , DegreePlan = 7251 ,Term =1, CreditID =563, Status =''C'' },</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2757,7 +2758,7 @@
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 4 , DegreePlan = 7251 ,Term =2 CreditID =560, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 4 , DegreePlan = 7251 ,Term =2, CreditID =560, Status =''A'' },</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2778,7 +2779,7 @@
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 5 , DegreePlan = 7251 ,Term =2 CreditID =664, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 5 , DegreePlan = 7251 ,Term =2, CreditID =664, Status =''A'' },</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2799,7 +2800,7 @@
       </c>
       <c r="F7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 6 , DegreePlan = 7251 ,Term =2 CreditID =6, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 6 , DegreePlan = 7251 ,Term =2, CreditID =6, Status =''A'' },</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2820,7 +2821,7 @@
       </c>
       <c r="F8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 7 , DegreePlan = 7251 ,Term =3 CreditID =618, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 7 , DegreePlan = 7251 ,Term =3, CreditID =618, Status =''P'' },</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,7 +2842,7 @@
       </c>
       <c r="F9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 8 , DegreePlan = 7251 ,Term =3 CreditID =691, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 8 , DegreePlan = 7251 ,Term =3, CreditID =691, Status =''P'' },</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2862,7 +2863,7 @@
       </c>
       <c r="F10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 9 , DegreePlan = 7251 ,Term =4 CreditID =692, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 9 , DegreePlan = 7251 ,Term =4, CreditID =692, Status =''P'' },</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2883,7 +2884,7 @@
       </c>
       <c r="F11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 10 , DegreePlan = 7251 ,Term =4 CreditID =1, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 10 , DegreePlan = 7251 ,Term =4, CreditID =1, Status =''P'' },</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2904,7 +2905,7 @@
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 11 , DegreePlan = 7251 ,Term =4 CreditID =2, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 11 , DegreePlan = 7251 ,Term =4, CreditID =2, Status =''P'' },</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,7 +2926,7 @@
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 12 , DegreePlan = 7251 ,Term =5 CreditID =555, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 12 , DegreePlan = 7251 ,Term =5, CreditID =555, Status =''P'' },</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,7 +2947,7 @@
       </c>
       <c r="F14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 13 , DegreePlan = 7252 ,Term =1 CreditID =460, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 13 , DegreePlan = 7252 ,Term =1, CreditID =460, Status =''C'' },</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2967,7 +2968,7 @@
       </c>
       <c r="F15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 14 , DegreePlan = 7252 ,Term =1 CreditID =542, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 14 , DegreePlan = 7252 ,Term =1, CreditID =542, Status =''C'' },</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2988,7 +2989,7 @@
       </c>
       <c r="F16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 15 , DegreePlan = 7252 ,Term =1 CreditID =563, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 15 , DegreePlan = 7252 ,Term =1, CreditID =563, Status =''C'' },</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3009,7 +3010,7 @@
       </c>
       <c r="F17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 16 , DegreePlan = 7252 ,Term =3 CreditID =560, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 16 , DegreePlan = 7252 ,Term =3, CreditID =560, Status =''C'' },</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3030,7 +3031,7 @@
       </c>
       <c r="F18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 17 , DegreePlan = 7252 ,Term =3 CreditID =664, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 17 , DegreePlan = 7252 ,Term =3, CreditID =664, Status =''A'' },</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3051,7 +3052,7 @@
       </c>
       <c r="F19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 18 , DegreePlan = 7252 ,Term =3 CreditID =6, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 18 , DegreePlan = 7252 ,Term =3, CreditID =6, Status =''A'' },</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3072,7 +3073,7 @@
       </c>
       <c r="F20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 19 , DegreePlan = 7252 ,Term =4 CreditID =691, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 19 , DegreePlan = 7252 ,Term =4, CreditID =691, Status =''A'' },</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3093,7 +3094,7 @@
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 20 , DegreePlan = 7252 ,Term =4 CreditID =618, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 20 , DegreePlan = 7252 ,Term =4, CreditID =618, Status =''P'' },</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3114,7 +3115,7 @@
       </c>
       <c r="F22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 21 , DegreePlan = 7252 ,Term =5 CreditID =692, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 21 , DegreePlan = 7252 ,Term =5, CreditID =692, Status =''P'' },</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3135,7 +3136,7 @@
       </c>
       <c r="F23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 22 , DegreePlan = 7252 ,Term =5 CreditID =1, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 22 , DegreePlan = 7252 ,Term =5, CreditID =1, Status =''P'' },</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3156,7 +3157,7 @@
       </c>
       <c r="F24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 23 , DegreePlan = 7252 ,Term =6 CreditID =555, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 23 , DegreePlan = 7252 ,Term =6, CreditID =555, Status =''P'' },</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3177,7 +3178,7 @@
       </c>
       <c r="F25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 24 , DegreePlan = 7252 ,Term =6 CreditID =2, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 24 , DegreePlan = 7252 ,Term =6, CreditID =2, Status =''P'' },</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3198,7 +3199,7 @@
       </c>
       <c r="F26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 25 , DegreePlan = 7255 ,Term =1 CreditID =460, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 25 , DegreePlan = 7255 ,Term =1, CreditID =460, Status =''C'' },</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3219,7 +3220,7 @@
       </c>
       <c r="F27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 26 , DegreePlan = 7255 ,Term =1 CreditID =542, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 26 , DegreePlan = 7255 ,Term =1, CreditID =542, Status =''C'' },</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3240,7 +3241,7 @@
       </c>
       <c r="F28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 27 , DegreePlan = 7255 ,Term =1 CreditID =563, Status =C}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 27 , DegreePlan = 7255 ,Term =1, CreditID =563, Status =''C'' },</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3261,7 +3262,7 @@
       </c>
       <c r="F29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 28 , DegreePlan = 7255 ,Term =2 CreditID =6, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 28 , DegreePlan = 7255 ,Term =2, CreditID =6, Status =''A'' },</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3282,7 +3283,7 @@
       </c>
       <c r="F30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 29 , DegreePlan = 7255 ,Term =2 CreditID =618, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 29 , DegreePlan = 7255 ,Term =2, CreditID =618, Status =''A'' },</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3303,7 +3304,7 @@
       </c>
       <c r="F31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 30 , DegreePlan = 7255 ,Term =2 CreditID =560, Status =A}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 30 , DegreePlan = 7255 ,Term =2, CreditID =560, Status =''A'' },</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3324,7 +3325,7 @@
       </c>
       <c r="F32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 31 , DegreePlan = 7255 ,Term =4 CreditID =691, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 31 , DegreePlan = 7255 ,Term =4, CreditID =691, Status =''P'' },</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3345,7 +3346,7 @@
       </c>
       <c r="F33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 32 , DegreePlan = 7255 ,Term =4 CreditID =1, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 32 , DegreePlan = 7255 ,Term =4, CreditID =1, Status =''P'' },</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3366,7 +3367,7 @@
       </c>
       <c r="F34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 33 , DegreePlan = 7255 ,Term =4 CreditID =2, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 33 , DegreePlan = 7255 ,Term =4, CreditID =2, Status =''P'' },</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3387,7 +3388,7 @@
       </c>
       <c r="F35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 34 , DegreePlan = 7255 ,Term =5 CreditID =555, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 34 , DegreePlan = 7255 ,Term =5, CreditID =555, Status =''P'' },</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3408,7 +3409,7 @@
       </c>
       <c r="F36" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 35 , DegreePlan = 7255 ,Term =5 CreditID =664, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 35 , DegreePlan = 7255 ,Term =5, CreditID =664, Status =''P'' },</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3429,7 +3430,7 @@
       </c>
       <c r="F37" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 36 , DegreePlan = 7255 ,Term =6 CreditID =692, Status =P}</v>
+        <v xml:space="preserve"> new Slot{SlotID = 36 , DegreePlan = 7255 ,Term =6, CreditID =692, Status =''P'' },</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Foreign keys are highlighted in the models
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
   <si>
     <t>DegreeID</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Snumber</t>
-  </si>
-  <si>
-    <t>DegreePlan</t>
   </si>
   <si>
     <t>Status</t>
@@ -776,10 +773,10 @@
         <v>46</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,10 +784,10 @@
         <v>533726</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="D2" s="3">
         <v>533726</v>
@@ -808,10 +805,10 @@
         <v>533490</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="D3" s="3">
         <v>533490</v>
@@ -829,10 +826,10 @@
         <v>533711</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="D4" s="3">
         <v>533711</v>
@@ -872,16 +869,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,7 +912,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,7 +929,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1014,7 +1011,7 @@
         <v>34</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,10 +1283,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1310,10 +1307,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -1341,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D49"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1361,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,7 +2094,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,7 +2120,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,10 +2167,10 @@
         <v>533490</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2188,10 +2185,10 @@
         <v>533490</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2206,10 +2203,10 @@
         <v>533711</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2243,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,22 +2256,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="F1" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2288,10 +2285,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="14" t="str">
         <f>" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;", "&amp;$D$1&amp;" = ''"&amp;D2&amp;"'',  "&amp;$E$1&amp;" =''"&amp;E2&amp;"'' },"</f>
@@ -2309,10 +2306,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="14" t="str">
         <f t="shared" ref="F3:F18" si="0">" new StudentTerm{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;", "&amp;$D$1&amp;" = ''"&amp;D3&amp;"'',  "&amp;$E$1&amp;" =''"&amp;E3&amp;"'' },"</f>
@@ -2330,10 +2327,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2351,10 +2348,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2372,10 +2369,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="F6" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2393,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2414,10 +2411,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2435,10 +2432,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2456,10 +2453,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2477,10 +2474,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2498,10 +2495,10 @@
         <v>6</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2519,10 +2516,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2540,10 +2537,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2561,10 +2558,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2582,10 +2579,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2603,10 +2600,10 @@
         <v>5</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2624,10 +2621,10 @@
         <v>6</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2644,13 +2641,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -2659,22 +2656,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,11 +2688,11 @@
         <v>460</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>" new Slot{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;", "&amp;$D$1&amp;" ="&amp;D2&amp;", "&amp;$E$1&amp;" ="&amp;"''"&amp;E2&amp;"'' },"</f>
-        <v xml:space="preserve"> new Slot{SlotID = 1 , DegreePlan = 7251 ,Term =1, CreditID =460, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 1 , DegreePlanID = 7251 ,Term =1, CreditID =460, Status =''C'' },</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2712,11 +2709,11 @@
         <v>542</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3" t="str">
         <f t="shared" ref="F3:F37" si="0">" new Slot{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;", "&amp;$D$1&amp;" ="&amp;D3&amp;", "&amp;$E$1&amp;" ="&amp;"''"&amp;E3&amp;"'' },"</f>
-        <v xml:space="preserve"> new Slot{SlotID = 2 , DegreePlan = 7251 ,Term =1, CreditID =542, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 2 , DegreePlanID = 7251 ,Term =1, CreditID =542, Status =''C'' },</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,11 +2730,11 @@
         <v>563</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 3 , DegreePlan = 7251 ,Term =1, CreditID =563, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 3 , DegreePlanID = 7251 ,Term =1, CreditID =563, Status =''C'' },</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2754,11 +2751,11 @@
         <v>560</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 4 , DegreePlan = 7251 ,Term =2, CreditID =560, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 4 , DegreePlanID = 7251 ,Term =2, CreditID =560, Status =''A'' },</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,11 +2772,11 @@
         <v>664</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 5 , DegreePlan = 7251 ,Term =2, CreditID =664, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 5 , DegreePlanID = 7251 ,Term =2, CreditID =664, Status =''A'' },</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,11 +2793,11 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 6 , DegreePlan = 7251 ,Term =2, CreditID =6, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 6 , DegreePlanID = 7251 ,Term =2, CreditID =6, Status =''A'' },</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2817,11 +2814,11 @@
         <v>618</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 7 , DegreePlan = 7251 ,Term =3, CreditID =618, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 7 , DegreePlanID = 7251 ,Term =3, CreditID =618, Status =''P'' },</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2838,11 +2835,11 @@
         <v>691</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 8 , DegreePlan = 7251 ,Term =3, CreditID =691, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 8 , DegreePlanID = 7251 ,Term =3, CreditID =691, Status =''P'' },</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2859,11 +2856,11 @@
         <v>692</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 9 , DegreePlan = 7251 ,Term =4, CreditID =692, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 9 , DegreePlanID = 7251 ,Term =4, CreditID =692, Status =''P'' },</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2880,11 +2877,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 10 , DegreePlan = 7251 ,Term =4, CreditID =1, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 10 , DegreePlanID = 7251 ,Term =4, CreditID =1, Status =''P'' },</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,11 +2898,11 @@
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 11 , DegreePlan = 7251 ,Term =4, CreditID =2, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 11 , DegreePlanID = 7251 ,Term =4, CreditID =2, Status =''P'' },</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,11 +2919,11 @@
         <v>555</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 12 , DegreePlan = 7251 ,Term =5, CreditID =555, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 12 , DegreePlanID = 7251 ,Term =5, CreditID =555, Status =''P'' },</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2943,11 +2940,11 @@
         <v>460</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 13 , DegreePlan = 7252 ,Term =1, CreditID =460, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 13 , DegreePlanID = 7252 ,Term =1, CreditID =460, Status =''C'' },</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2964,11 +2961,11 @@
         <v>542</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 14 , DegreePlan = 7252 ,Term =1, CreditID =542, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 14 , DegreePlanID = 7252 ,Term =1, CreditID =542, Status =''C'' },</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,11 +2982,11 @@
         <v>563</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 15 , DegreePlan = 7252 ,Term =1, CreditID =563, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 15 , DegreePlanID = 7252 ,Term =1, CreditID =563, Status =''C'' },</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3006,11 +3003,11 @@
         <v>560</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 16 , DegreePlan = 7252 ,Term =3, CreditID =560, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 16 , DegreePlanID = 7252 ,Term =3, CreditID =560, Status =''C'' },</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3027,11 +3024,11 @@
         <v>664</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 17 , DegreePlan = 7252 ,Term =3, CreditID =664, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 17 , DegreePlanID = 7252 ,Term =3, CreditID =664, Status =''A'' },</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3048,11 +3045,11 @@
         <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 18 , DegreePlan = 7252 ,Term =3, CreditID =6, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 18 , DegreePlanID = 7252 ,Term =3, CreditID =6, Status =''A'' },</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,11 +3066,11 @@
         <v>691</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 19 , DegreePlan = 7252 ,Term =4, CreditID =691, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 19 , DegreePlanID = 7252 ,Term =4, CreditID =691, Status =''A'' },</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3090,11 +3087,11 @@
         <v>618</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 20 , DegreePlan = 7252 ,Term =4, CreditID =618, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 20 , DegreePlanID = 7252 ,Term =4, CreditID =618, Status =''P'' },</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3111,11 +3108,11 @@
         <v>692</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 21 , DegreePlan = 7252 ,Term =5, CreditID =692, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 21 , DegreePlanID = 7252 ,Term =5, CreditID =692, Status =''P'' },</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3132,11 +3129,11 @@
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 22 , DegreePlan = 7252 ,Term =5, CreditID =1, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 22 , DegreePlanID = 7252 ,Term =5, CreditID =1, Status =''P'' },</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3153,11 +3150,11 @@
         <v>555</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 23 , DegreePlan = 7252 ,Term =6, CreditID =555, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 23 , DegreePlanID = 7252 ,Term =6, CreditID =555, Status =''P'' },</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3174,11 +3171,11 @@
         <v>2</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 24 , DegreePlan = 7252 ,Term =6, CreditID =2, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 24 , DegreePlanID = 7252 ,Term =6, CreditID =2, Status =''P'' },</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3195,11 +3192,11 @@
         <v>460</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 25 , DegreePlan = 7255 ,Term =1, CreditID =460, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 25 , DegreePlanID = 7255 ,Term =1, CreditID =460, Status =''C'' },</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3216,11 +3213,11 @@
         <v>542</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 26 , DegreePlan = 7255 ,Term =1, CreditID =542, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 26 , DegreePlanID = 7255 ,Term =1, CreditID =542, Status =''C'' },</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3237,11 +3234,11 @@
         <v>563</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 27 , DegreePlan = 7255 ,Term =1, CreditID =563, Status =''C'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 27 , DegreePlanID = 7255 ,Term =1, CreditID =563, Status =''C'' },</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3258,11 +3255,11 @@
         <v>6</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 28 , DegreePlan = 7255 ,Term =2, CreditID =6, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 28 , DegreePlanID = 7255 ,Term =2, CreditID =6, Status =''A'' },</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3279,11 +3276,11 @@
         <v>618</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 29 , DegreePlan = 7255 ,Term =2, CreditID =618, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 29 , DegreePlanID = 7255 ,Term =2, CreditID =618, Status =''A'' },</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3300,11 +3297,11 @@
         <v>560</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 30 , DegreePlan = 7255 ,Term =2, CreditID =560, Status =''A'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 30 , DegreePlanID = 7255 ,Term =2, CreditID =560, Status =''A'' },</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3321,11 +3318,11 @@
         <v>691</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 31 , DegreePlan = 7255 ,Term =4, CreditID =691, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 31 , DegreePlanID = 7255 ,Term =4, CreditID =691, Status =''P'' },</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3342,11 +3339,11 @@
         <v>1</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 32 , DegreePlan = 7255 ,Term =4, CreditID =1, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 32 , DegreePlanID = 7255 ,Term =4, CreditID =1, Status =''P'' },</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3363,11 +3360,11 @@
         <v>2</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 33 , DegreePlan = 7255 ,Term =4, CreditID =2, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 33 , DegreePlanID = 7255 ,Term =4, CreditID =2, Status =''P'' },</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3384,11 +3381,11 @@
         <v>555</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 34 , DegreePlan = 7255 ,Term =5, CreditID =555, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 34 , DegreePlanID = 7255 ,Term =5, CreditID =555, Status =''P'' },</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3405,11 +3402,11 @@
         <v>664</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 35 , DegreePlan = 7255 ,Term =5, CreditID =664, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 35 , DegreePlanID = 7255 ,Term =5, CreditID =664, Status =''P'' },</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3426,11 +3423,11 @@
         <v>692</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Slot{SlotID = 36 , DegreePlan = 7255 ,Term =6, CreditID =692, Status =''P'' },</v>
+        <v xml:space="preserve"> new Slot{SlotID = 36 , DegreePlanID = 7255 ,Term =6, CreditID =692, Status =''P'' },</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated DbInitializer.cs for Student and Studentterms
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +755,8 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="109.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -852,7 +853,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2095,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2242,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Content in the SlotController.cs
</commit_message>
<xml_diff>
--- a/DegreePlan.xlsx
+++ b/DegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533490\Documents\44663\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533711\Desktop\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -746,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2241,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>